<commit_message>
updated examples created fake data sets
</commit_message>
<xml_diff>
--- a/inst/examples/keyFile.xlsx
+++ b/inst/examples/keyFile.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\projects\wurmc_(mverouden_GITHUB)\inst\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5376D82A-768E-4A30-ADAB-DD63CE002A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D8C060-8BF5-4062-86A9-07A7C740D020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21150" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="antwoorden" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="30">
   <si>
     <t>Q01</t>
   </si>
@@ -121,13 +121,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,8 +157,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,16 +474,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:Z5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="26" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="1009" width="10.625" customWidth="1"/>
-    <col min="1010" max="1025" width="8.375" customWidth="1"/>
+    <col min="27" max="1005" width="10.625" customWidth="1"/>
+    <col min="1006" max="1021" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -565,80 +572,320 @@
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" t="s">
-        <v>25</v>
-      </c>
-      <c r="W2" t="s">
-        <v>27</v>
-      </c>
-      <c r="X2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>28</v>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>